<commit_message>
A lot of changes, need few tweeks to utility func
</commit_message>
<xml_diff>
--- a/data/_combined_datasets.xlsx
+++ b/data/_combined_datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmchrist\Desktop\ABM\Assignment\ABM-Housing-Pricing\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E844063F-B838-46B9-B675-904EFB09BAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F14C42-9B9B-4F48-A452-8915F149854D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1071,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ8"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>

</xml_diff>